<commit_message>
implemented a preliminary version of eligibility rules.
</commit_message>
<xml_diff>
--- a/src/main/resources/eligibility_rules.xlsx
+++ b/src/main/resources/eligibility_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Projects/git/DecisionEngine/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85506CA-75BC-C642-BE3B-57814193A348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB98C9D-6A9E-7F43-8D71-D400E174FDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="7020" windowWidth="28040" windowHeight="17440" xr2:uid="{90C67E40-D382-414D-9199-6A3F4850161E}"/>
+    <workbookView xWindow="15880" yWindow="11020" windowWidth="47040" windowHeight="17440" xr2:uid="{90C67E40-D382-414D-9199-6A3F4850161E}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,52 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Li Lin</author>
+  </authors>
+  <commentList>
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{A475CF32-504E-F54C-86F9-6F831D6135EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Li Lin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the purpose of this column is to declare variable $d so that it can be used later in the action. the falg is just dummy
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>RuleSet</t>
   </si>
@@ -50,12 +94,6 @@
     <t>CONDITION</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>OwnershipType</t>
-  </si>
-  <si>
     <t>Rule Name</t>
   </si>
   <si>
@@ -65,59 +103,131 @@
     <t>simple eligibility decision table</t>
   </si>
   <si>
-    <t>Eligibility</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>$customer:Customer</t>
-  </si>
-  <si>
-    <t>CA not ok</t>
-  </si>
-  <si>
-    <t>ZZ ok</t>
-  </si>
-  <si>
-    <t>CustomerTypeCode</t>
-  </si>
-  <si>
-    <t>"NO"</t>
-  </si>
-  <si>
-    <t>"YES"</t>
-  </si>
-  <si>
     <t>net.vino9.demo.decisionengine</t>
   </si>
   <si>
-    <t>net.vino9.demo.decisionengine.Customer</t>
-  </si>
-  <si>
-    <t>$customer.setEligibility($param);</t>
-  </si>
-  <si>
-    <t>"INDIVIDUAL"</t>
-  </si>
-  <si>
-    <t>"CA"</t>
-  </si>
-  <si>
-    <t>"ZZ"</t>
-  </si>
-  <si>
     <t>ownershipType in ($param)</t>
   </si>
   <si>
-    <t>customerTypeCode == $param</t>
+    <t>ineligible customer types</t>
+  </si>
+  <si>
+    <t>"CA","CB","CC","CD","DA","EA"</t>
+  </si>
+  <si>
+    <t>Customer Type Code</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Ownership</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>net.vino9.demo.decisionengine.models.Account, net.vino9.demo.decisionengine.models.Customer, net.vino9.demo.decisionengine.models.Decision</t>
+  </si>
+  <si>
+    <t>$cust:Customer</t>
+  </si>
+  <si>
+    <t>$acc:Account</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Eligible </t>
+  </si>
+  <si>
+    <t>Account Eligible</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>"Individual","Payroll","Payroll-like"</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Deal</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>CLSB</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>card closed by bank</t>
+  </si>
+  <si>
+    <t>open saving account</t>
+  </si>
+  <si>
+    <t>closed saving account</t>
+  </si>
+  <si>
+    <t>open deal account</t>
+  </si>
+  <si>
+    <t>typeCode in ( $param)</t>
+  </si>
+  <si>
+    <t>productType == "$param"</t>
+  </si>
+  <si>
+    <t>status == "$param"</t>
+  </si>
+  <si>
+    <t>productCode  == "$param"</t>
+  </si>
+  <si>
+    <t>$d:Decision</t>
+  </si>
+  <si>
+    <t>$d.addAccount($acc.getAccountNumber(), "$param");</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>$d.markCustomerIneligible("$param");</t>
+  </si>
+  <si>
+    <t>flag == $param</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,6 +262,19 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -229,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -247,6 +370,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -565,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183D81F8-9B58-004B-9BA1-7CEAD6B70474}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183D81F8-9B58-004B-9BA1-7CEAD6B70474}">
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,50 +706,68 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="3" max="3" width="53.83203125" customWidth="1"/>
-    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
+    <col min="5" max="6" width="27.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="37.5" customWidth="1"/>
+    <col min="9" max="9" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>3</v>
@@ -628,73 +775,203 @@
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="11">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>